<commit_message>
Documento Inicial Herramientas y Tecnologias
</commit_message>
<xml_diff>
--- a/Nomenclaturas.xlsx
+++ b/Nomenclaturas.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eduar\Documents\GitHub\Testify\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19420" windowHeight="8910"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19425" windowHeight="8910"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Codigo</t>
   </si>
@@ -106,13 +111,16 @@
   </si>
   <si>
     <t>Plan de Iteración</t>
+  </si>
+  <si>
+    <t>Herramientas y Tecnologias</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,7 +211,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -238,7 +246,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -415,23 +423,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -439,7 +447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -447,7 +455,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -455,7 +463,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -463,7 +471,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -471,91 +479,94 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
Documentación - Actualización Plan SQA
Se actualiza el plan de SQA, se añade plan de gestión de configuración.
</commit_message>
<xml_diff>
--- a/Nomenclaturas.xlsx
+++ b/Nomenclaturas.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eduar\Documents\GitHub\Testify\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19425" windowHeight="8910"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19420" windowHeight="8910"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Codigo</t>
   </si>
@@ -114,13 +109,16 @@
   </si>
   <si>
     <t>Herramientas y Tecnologias</t>
+  </si>
+  <si>
+    <t>Plan de Gestión de la configuración</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -211,7 +209,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -246,7 +244,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -423,23 +421,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -447,7 +445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -455,7 +453,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -463,7 +461,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -471,7 +469,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -479,7 +477,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -487,7 +485,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -495,7 +493,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -503,70 +501,73 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1">
       <c r="A17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1">
       <c r="A18" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1">
       <c r="A19" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1">
       <c r="A20" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1">
       <c r="A21" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
Documentación - Actualización nomenclatura
Se realiza actualización de la plantilla de excel con nomenclatura de nombres basados en el estándar OSLO.
</commit_message>
<xml_diff>
--- a/Nomenclaturas.xlsx
+++ b/Nomenclaturas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Proyecto\LDS\Testify\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53997F9C-0006-4DE3-99BA-779DF0424E33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A97FA5B-0450-4463-BAA3-645C18667B6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="63">
   <si>
     <t>Codigo</t>
   </si>
   <si>
-    <t>Documento</t>
-  </si>
-  <si>
     <t>Plan de Proyecto</t>
   </si>
   <si>
@@ -190,6 +187,33 @@
   </si>
   <si>
     <t>Informe de Revisión Técnica Formal</t>
+  </si>
+  <si>
+    <t>Fase iteración</t>
+  </si>
+  <si>
+    <t>E212</t>
+  </si>
+  <si>
+    <t>E213</t>
+  </si>
+  <si>
+    <t>E214</t>
+  </si>
+  <si>
+    <t>E215</t>
+  </si>
+  <si>
+    <t>E216</t>
+  </si>
+  <si>
+    <t>E217</t>
+  </si>
+  <si>
+    <t>E218</t>
+  </si>
+  <si>
+    <t>E219</t>
   </si>
 </sst>
 </file>
@@ -211,15 +235,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -227,12 +263,129 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -513,244 +666,272 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="12" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="C6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="C7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="C9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="C14" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="C15" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" s="4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="C16" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" s="6" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="C17" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" s="6" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="C18" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="B20" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B20" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>14</v>
-      </c>
-      <c r="B22" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>16</v>
-      </c>
-      <c r="B24" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>17</v>
-      </c>
-      <c r="B25" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>23</v>
-      </c>
-    </row>
+      <c r="C20" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="23" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Documentación - Actualización de reuniones
Se añaden los documentos de las reuniones 13 y 14 correspondiente a la fase de elaboración iteración 2. Se realizan correcciones ortográficas y gestión SQA sobre resumen de reunión 12.
</commit_message>
<xml_diff>
--- a/Nomenclaturas.xlsx
+++ b/Nomenclaturas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Proyecto\LDS\Testify\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F49B27-E9A6-4C59-A756-479096D634D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BE9F746-6FE9-47DE-B10C-7FBF2E3FA66B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="94">
   <si>
     <t>Codigo</t>
   </si>
@@ -291,13 +291,22 @@
     <t>IN17</t>
   </si>
   <si>
-    <t>Documento</t>
-  </si>
-  <si>
     <t>E220</t>
   </si>
   <si>
     <t>E221</t>
+  </si>
+  <si>
+    <t>E222</t>
+  </si>
+  <si>
+    <t>Inicio</t>
+  </si>
+  <si>
+    <t>Elaboración Iteración 1</t>
+  </si>
+  <si>
+    <t>Elaboración Iteración 2</t>
   </si>
 </sst>
 </file>
@@ -880,8 +889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -896,19 +905,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="C1" s="15" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="16" t="s">
-        <v>88</v>
+      <c r="F1" s="9" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="29.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -1228,6 +1237,8 @@
       <c r="F20" s="2"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="10"/>
+      <c r="B21" s="14"/>
       <c r="C21" s="19" t="s">
         <v>62</v>
       </c>
@@ -1235,11 +1246,13 @@
         <v>74</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F21" s="2"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="10"/>
+      <c r="B22" s="14"/>
       <c r="C22" s="19" t="s">
         <v>63</v>
       </c>
@@ -1247,17 +1260,23 @@
         <v>75</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F22" s="2"/>
     </row>
     <row r="23" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="10"/>
+      <c r="B23" s="14"/>
       <c r="C23" s="19" t="s">
         <v>64</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>76</v>
       </c>
+      <c r="E23" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>

</xml_diff>

<commit_message>
Documentación - Revisión SQA prototipo
Se realizan correcciones al prototipo funcional, se corrigen hipervínculos, encabezados y formato visual, se añade el nombre basado en el estándar OSLO definido por el equipo de desarrollo.

Co-Authored-By: Proypb20 <34356468+Proypb20@users.noreply.github.com>
Co-Authored-By: malebea30 <179352973+malebea30@users.noreply.github.com>
Co-Authored-By: vhalianna <44414354+vhalianna@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Nomenclaturas.xlsx
+++ b/Nomenclaturas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Proyecto\LDS\Testify\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BE9F746-6FE9-47DE-B10C-7FBF2E3FA66B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00539D98-A9C4-4023-B116-8259CE38356D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="95">
   <si>
     <t>Codigo</t>
   </si>
@@ -307,6 +307,9 @@
   </si>
   <si>
     <t>Elaboración Iteración 2</t>
+  </si>
+  <si>
+    <t>Prototipo Funcional Testify</t>
   </si>
 </sst>
 </file>
@@ -890,14 +893,14 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="22.85546875" customWidth="1"/>
     <col min="4" max="4" width="22.5703125" customWidth="1"/>
-    <col min="6" max="6" width="23" customWidth="1"/>
+    <col min="6" max="6" width="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1076,7 +1079,9 @@
       <c r="E9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="2"/>
+      <c r="F9" s="2" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="10" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">

</xml_diff>

<commit_message>
E209- Modelo de Datos
</commit_message>
<xml_diff>
--- a/Nomenclaturas.xlsx
+++ b/Nomenclaturas.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Proyecto\LDS\Testify\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eduar\Documents\GitHub\Testify\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00539D98-A9C4-4023-B116-8259CE38356D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="96">
   <si>
     <t>Codigo</t>
   </si>
@@ -310,12 +309,15 @@
   </si>
   <si>
     <t>Prototipo Funcional Testify</t>
+  </si>
+  <si>
+    <t>Modelo de Datos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -889,11 +891,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1099,7 +1101,9 @@
       <c r="E10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="2"/>
+      <c r="F10" s="2" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>

</xml_diff>

<commit_message>
Documentación - Confección RTF plan de pruebas.
Se realiza la confección correspondiente a la revisión técnica formal del plan de pruebas y se añade al seguimiento para nomenclaturas de nombres.
</commit_message>
<xml_diff>
--- a/Nomenclaturas.xlsx
+++ b/Nomenclaturas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Proyecto\LDS\Testify\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEB25AAB-CEA5-402D-A394-9D3D24253E00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B38B6B1-D76A-4D50-BC7D-E7A69580CFF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="99">
   <si>
     <t>Codigo</t>
   </si>
@@ -915,14 +915,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="22.85546875" customWidth="1"/>
-    <col min="4" max="4" width="22.5703125" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" customWidth="1"/>
     <col min="6" max="6" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1174,7 +1174,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="14"/>
       <c r="C14" s="19" t="s">
@@ -1186,7 +1186,9 @@
       <c r="E14" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="F14" s="2"/>
+      <c r="F14" s="3" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>

</xml_diff>

<commit_message>
Se actualizo el documento de nomenclaturas
Se agrego dos documentos con el E214 y E215 para los archivos de análisis y seguimiento de riesgos
</commit_message>
<xml_diff>
--- a/Nomenclaturas.xlsx
+++ b/Nomenclaturas.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Valeria\Documents\Oslo\Testify\Testify\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malen\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{32A38CAD-9CC9-4B2B-9F4C-3E5837E85EC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="102">
   <si>
     <t>Codigo</t>
   </si>
@@ -337,19 +327,16 @@
     <t>C101</t>
   </si>
   <si>
-    <t>C102</t>
-  </si>
-  <si>
-    <t>C103</t>
-  </si>
-  <si>
-    <t>CU01 - CRUD Escenario</t>
+    <t>Identificación, Evaluación y análisis de riesgos - Anexo II 09-10-2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Seguimiento de Riesgos III 09-10-2024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -704,7 +691,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -739,7 +726,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -923,21 +910,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="22.85546875" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" customWidth="1"/>
-    <col min="6" max="6" width="27.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.88671875" customWidth="1"/>
+    <col min="4" max="4" width="26.88671875" customWidth="1"/>
+    <col min="6" max="6" width="57" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -957,7 +944,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="29.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="29.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>79</v>
       </c>
@@ -979,11 +966,8 @@
       <c r="G2" t="s">
         <v>99</v>
       </c>
-      <c r="H2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>80</v>
       </c>
@@ -1002,14 +986,8 @@
       <c r="F3" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="G3" t="s">
-        <v>100</v>
-      </c>
-      <c r="H3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>81</v>
       </c>
@@ -1028,11 +1006,8 @@
       <c r="F4" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>82</v>
       </c>
@@ -1052,7 +1027,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>83</v>
       </c>
@@ -1072,7 +1047,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>84</v>
       </c>
@@ -1092,7 +1067,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>85</v>
       </c>
@@ -1112,7 +1087,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>86</v>
       </c>
@@ -1132,7 +1107,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>87</v>
       </c>
@@ -1152,7 +1127,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="10"/>
       <c r="B11" s="14"/>
       <c r="C11" s="19" t="s">
@@ -1168,7 +1143,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="10"/>
       <c r="B12" s="14"/>
       <c r="C12" s="19" t="s">
@@ -1184,7 +1159,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
       <c r="B13" s="14"/>
       <c r="C13" s="19" t="s">
@@ -1200,7 +1175,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
       <c r="B14" s="14"/>
       <c r="C14" s="19" t="s">
@@ -1216,7 +1191,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
       <c r="B15" s="14"/>
       <c r="C15" s="19" t="s">
@@ -1228,9 +1203,11 @@
       <c r="E15" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F15" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="10"/>
       <c r="B16" s="14"/>
       <c r="C16" s="19" t="s">
@@ -1242,9 +1219,11 @@
       <c r="E16" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F16" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10"/>
       <c r="B17" s="14"/>
       <c r="C17" s="19" t="s">
@@ -1258,7 +1237,7 @@
       </c>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10"/>
       <c r="B18" s="14"/>
       <c r="C18" s="19" t="s">
@@ -1272,7 +1251,7 @@
       </c>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10"/>
       <c r="B19" s="14"/>
       <c r="C19" s="19" t="s">
@@ -1286,7 +1265,7 @@
       </c>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="10"/>
       <c r="B20" s="14"/>
       <c r="C20" s="19" t="s">
@@ -1300,7 +1279,7 @@
       </c>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="10"/>
       <c r="B21" s="14"/>
       <c r="C21" s="19" t="s">
@@ -1314,7 +1293,7 @@
       </c>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="10"/>
       <c r="B22" s="14"/>
       <c r="C22" s="19" t="s">
@@ -1328,7 +1307,7 @@
       </c>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10"/>
       <c r="B23" s="14"/>
       <c r="C23" s="19" t="s">
@@ -1342,7 +1321,7 @@
       </c>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Documentación - Revisión SQA rutinaria
Se realiza revisión rutinaria sobre documentos de apoyo, se realizan modificaciones de nombres acorde a la nomenclatura estándar definida OSLO, se realiza limpieza de archivos temporales en repositorio Registro_Reuniones.
</commit_message>
<xml_diff>
--- a/Nomenclaturas.xlsx
+++ b/Nomenclaturas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malen\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Proyecto\LDS\Testify\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{32A38CAD-9CC9-4B2B-9F4C-3E5837E85EC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8A63667-4802-4FA8-B544-ABC6C689137D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="119">
   <si>
     <t>Codigo</t>
   </si>
@@ -331,6 +331,57 @@
   </si>
   <si>
     <t xml:space="preserve"> Seguimiento de Riesgos III 09-10-2024</t>
+  </si>
+  <si>
+    <t>Construcción Iteración 1</t>
+  </si>
+  <si>
+    <t>CRUD Escenario.docx</t>
+  </si>
+  <si>
+    <t>C102</t>
+  </si>
+  <si>
+    <t>C103</t>
+  </si>
+  <si>
+    <t>Arquitectura del Sistema</t>
+  </si>
+  <si>
+    <t>C104</t>
+  </si>
+  <si>
+    <t>C105</t>
+  </si>
+  <si>
+    <t>C106</t>
+  </si>
+  <si>
+    <t>C107</t>
+  </si>
+  <si>
+    <t>C108</t>
+  </si>
+  <si>
+    <t>C109</t>
+  </si>
+  <si>
+    <t>C110</t>
+  </si>
+  <si>
+    <t>C111</t>
+  </si>
+  <si>
+    <t>C112</t>
+  </si>
+  <si>
+    <t>C113</t>
+  </si>
+  <si>
+    <t>C114</t>
+  </si>
+  <si>
+    <t>C115</t>
   </si>
 </sst>
 </file>
@@ -911,20 +962,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.88671875" customWidth="1"/>
-    <col min="4" max="4" width="26.88671875" customWidth="1"/>
-    <col min="6" max="6" width="57" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="3" max="3" width="7.140625" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" customWidth="1"/>
+    <col min="6" max="6" width="29" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" customWidth="1"/>
+    <col min="8" max="8" width="33.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -943,8 +999,14 @@
       <c r="F1" s="9" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="29.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="G1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="29.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>79</v>
       </c>
@@ -963,11 +1025,14 @@
       <c r="F2" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="12" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H2" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>80</v>
       </c>
@@ -986,8 +1051,14 @@
       <c r="F3" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G3" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>81</v>
       </c>
@@ -1006,8 +1077,14 @@
       <c r="F4" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G4" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>82</v>
       </c>
@@ -1026,8 +1103,12 @@
       <c r="F5" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G5" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="H5" s="10"/>
+    </row>
+    <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>83</v>
       </c>
@@ -1046,8 +1127,12 @@
       <c r="F6" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G6" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="H6" s="10"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>84</v>
       </c>
@@ -1066,8 +1151,12 @@
       <c r="F7" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G7" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="H7" s="10"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>85</v>
       </c>
@@ -1086,8 +1175,12 @@
       <c r="F8" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G8" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="H8" s="10"/>
+    </row>
+    <row r="9" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>86</v>
       </c>
@@ -1106,8 +1199,12 @@
       <c r="F9" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G9" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="H9" s="10"/>
+    </row>
+    <row r="10" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>87</v>
       </c>
@@ -1126,8 +1223,12 @@
       <c r="F10" s="2" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G10" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="H10" s="10"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
       <c r="B11" s="14"/>
       <c r="C11" s="19" t="s">
@@ -1142,8 +1243,12 @@
       <c r="F11" s="2" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G11" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="H11" s="10"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="B12" s="14"/>
       <c r="C12" s="19" t="s">
@@ -1158,8 +1263,12 @@
       <c r="F12" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G12" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="H12" s="10"/>
+    </row>
+    <row r="13" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="14"/>
       <c r="C13" s="19" t="s">
@@ -1174,8 +1283,12 @@
       <c r="F13" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G13" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="H13" s="10"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="14"/>
       <c r="C14" s="19" t="s">
@@ -1190,8 +1303,12 @@
       <c r="F14" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G14" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="H14" s="10"/>
+    </row>
+    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="14"/>
       <c r="C15" s="19" t="s">
@@ -1203,11 +1320,15 @@
       <c r="E15" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="3" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G15" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="H15" s="10"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="B16" s="14"/>
       <c r="C16" s="19" t="s">
@@ -1219,11 +1340,15 @@
       <c r="E16" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="3" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G16" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="H16" s="10"/>
+    </row>
+    <row r="17" spans="1:8" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
       <c r="B17" s="14"/>
       <c r="C17" s="19" t="s">
@@ -1236,8 +1361,10 @@
         <v>58</v>
       </c>
       <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+    </row>
+    <row r="18" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="14"/>
       <c r="C18" s="19" t="s">
@@ -1250,8 +1377,10 @@
         <v>59</v>
       </c>
       <c r="F18" s="2"/>
-    </row>
-    <row r="19" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G18" s="10"/>
+      <c r="H18" s="10"/>
+    </row>
+    <row r="19" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
       <c r="B19" s="14"/>
       <c r="C19" s="19" t="s">
@@ -1264,8 +1393,10 @@
         <v>60</v>
       </c>
       <c r="F19" s="2"/>
-    </row>
-    <row r="20" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+    </row>
+    <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
       <c r="B20" s="14"/>
       <c r="C20" s="19" t="s">
@@ -1278,8 +1409,10 @@
         <v>61</v>
       </c>
       <c r="F20" s="2"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
       <c r="B21" s="14"/>
       <c r="C21" s="19" t="s">
@@ -1292,8 +1425,10 @@
         <v>88</v>
       </c>
       <c r="F21" s="2"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
       <c r="B22" s="14"/>
       <c r="C22" s="19" t="s">
@@ -1306,8 +1441,10 @@
         <v>89</v>
       </c>
       <c r="F22" s="2"/>
-    </row>
-    <row r="23" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+    </row>
+    <row r="23" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
       <c r="B23" s="14"/>
       <c r="C23" s="19" t="s">
@@ -1320,8 +1457,10 @@
         <v>90</v>
       </c>
       <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+    </row>
+    <row r="24" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Documentación - Preparación entorno SQA
Se realiza la preparación del entorno de SQA correspondiente a la fase de construcción.
</commit_message>
<xml_diff>
--- a/Nomenclaturas.xlsx
+++ b/Nomenclaturas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Proyecto\LDS\Testify\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB73846-3DAB-43BD-A971-F1CA13BA5808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C39FD03-2A7F-449F-AB03-0AD23B8337FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -968,7 +968,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Documento de Riesgos C1-Cierre 1
Se realizo el análisis de los riesgos al cierre de la iteración 1 de C1 y se actualizo en nomenclador
</commit_message>
<xml_diff>
--- a/Nomenclaturas.xlsx
+++ b/Nomenclaturas.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Valeria\Documents\Oslo\Testify\Testify\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malen\OneDrive\Desktop\LDS\Testify\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C93C6DD-AEB5-4156-9129-5C36492B3374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="123">
   <si>
     <t>Codigo</t>
   </si>
@@ -387,12 +388,18 @@
   </si>
   <si>
     <t>CRUD Iteración</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Identificación, Evaluación y análisis de riesgos - Anexo II 27-10-2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Seguimiento de Riesgos IIII 27-10-2024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -659,7 +666,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -687,6 +694,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -966,26 +976,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" customWidth="1"/>
-    <col min="3" max="3" width="7.140625" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" customWidth="1"/>
+    <col min="2" max="2" width="22.88671875" customWidth="1"/>
+    <col min="3" max="3" width="7.109375" customWidth="1"/>
+    <col min="4" max="4" width="26.88671875" customWidth="1"/>
+    <col min="5" max="5" width="7.109375" customWidth="1"/>
     <col min="6" max="6" width="29" customWidth="1"/>
-    <col min="7" max="7" width="7.140625" customWidth="1"/>
-    <col min="8" max="8" width="33.140625" customWidth="1"/>
+    <col min="7" max="7" width="7.109375" customWidth="1"/>
+    <col min="8" max="8" width="33.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1011,7 +1021,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="29.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="29.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>79</v>
       </c>
@@ -1037,7 +1047,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>80</v>
       </c>
@@ -1063,7 +1073,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>81</v>
       </c>
@@ -1089,7 +1099,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>82</v>
       </c>
@@ -1115,7 +1125,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>83</v>
       </c>
@@ -1141,7 +1151,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>84</v>
       </c>
@@ -1163,9 +1173,11 @@
       <c r="G7" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="H7" s="10"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H7" s="21" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>85</v>
       </c>
@@ -1187,9 +1199,11 @@
       <c r="G8" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="H8" s="10"/>
-    </row>
-    <row r="9" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H8" s="10" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>86</v>
       </c>
@@ -1213,7 +1227,7 @@
       </c>
       <c r="H9" s="10"/>
     </row>
-    <row r="10" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>87</v>
       </c>
@@ -1237,7 +1251,7 @@
       </c>
       <c r="H10" s="10"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="10"/>
       <c r="B11" s="14"/>
       <c r="C11" s="19" t="s">
@@ -1257,7 +1271,7 @@
       </c>
       <c r="H11" s="10"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="10"/>
       <c r="B12" s="14"/>
       <c r="C12" s="19" t="s">
@@ -1277,7 +1291,7 @@
       </c>
       <c r="H12" s="10"/>
     </row>
-    <row r="13" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
       <c r="B13" s="14"/>
       <c r="C13" s="19" t="s">
@@ -1297,7 +1311,7 @@
       </c>
       <c r="H13" s="10"/>
     </row>
-    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="10"/>
       <c r="B14" s="14"/>
       <c r="C14" s="19" t="s">
@@ -1317,7 +1331,7 @@
       </c>
       <c r="H14" s="10"/>
     </row>
-    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
       <c r="B15" s="14"/>
       <c r="C15" s="19" t="s">
@@ -1337,7 +1351,7 @@
       </c>
       <c r="H15" s="10"/>
     </row>
-    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="10"/>
       <c r="B16" s="14"/>
       <c r="C16" s="19" t="s">
@@ -1357,7 +1371,7 @@
       </c>
       <c r="H16" s="10"/>
     </row>
-    <row r="17" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10"/>
       <c r="B17" s="14"/>
       <c r="C17" s="19" t="s">
@@ -1375,7 +1389,7 @@
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
     </row>
-    <row r="18" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10"/>
       <c r="B18" s="14"/>
       <c r="C18" s="19" t="s">
@@ -1391,7 +1405,7 @@
       <c r="G18" s="10"/>
       <c r="H18" s="10"/>
     </row>
-    <row r="19" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10"/>
       <c r="B19" s="14"/>
       <c r="C19" s="19" t="s">
@@ -1407,7 +1421,7 @@
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
     </row>
-    <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="10"/>
       <c r="B20" s="14"/>
       <c r="C20" s="19" t="s">
@@ -1423,7 +1437,7 @@
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="10"/>
       <c r="B21" s="14"/>
       <c r="C21" s="19" t="s">
@@ -1439,7 +1453,7 @@
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="10"/>
       <c r="B22" s="14"/>
       <c r="C22" s="19" t="s">
@@ -1455,7 +1469,7 @@
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
     </row>
-    <row r="23" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10"/>
       <c r="B23" s="14"/>
       <c r="C23" s="19" t="s">
@@ -1471,7 +1485,7 @@
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
     </row>
-    <row r="24" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Documentación - Revisión SQA
Se realiza revisión SQA sobre el repositorio resumen de reuniones, se añaden los documentos faltantes y se actualiza el archivo excel de nomenclatura de nombres.
</commit_message>
<xml_diff>
--- a/Nomenclaturas.xlsx
+++ b/Nomenclaturas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malen\OneDrive\Desktop\LDS\Testify\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Proyecto\LDS\Testify\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C93C6DD-AEB5-4156-9129-5C36492B3374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1A6183E-0C85-480C-ACE0-06221DACD419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="126">
   <si>
     <t>Codigo</t>
   </si>
@@ -394,6 +394,15 @@
   </si>
   <si>
     <t xml:space="preserve"> Seguimiento de Riesgos IIII 27-10-2024</t>
+  </si>
+  <si>
+    <t>Resumen de Reunión 19</t>
+  </si>
+  <si>
+    <t>Resumen de Reunión 20</t>
+  </si>
+  <si>
+    <t>Resumen de Reunión 21</t>
   </si>
 </sst>
 </file>
@@ -979,23 +988,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
-    <col min="2" max="2" width="22.88671875" customWidth="1"/>
-    <col min="3" max="3" width="7.109375" customWidth="1"/>
-    <col min="4" max="4" width="26.88671875" customWidth="1"/>
-    <col min="5" max="5" width="7.109375" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="3" max="3" width="7.140625" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" customWidth="1"/>
     <col min="6" max="6" width="29" customWidth="1"/>
-    <col min="7" max="7" width="7.109375" customWidth="1"/>
-    <col min="8" max="8" width="33.109375" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" customWidth="1"/>
+    <col min="8" max="8" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1021,7 +1030,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="29.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="29.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>79</v>
       </c>
@@ -1047,7 +1056,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>80</v>
       </c>
@@ -1073,7 +1082,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>81</v>
       </c>
@@ -1099,7 +1108,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>82</v>
       </c>
@@ -1125,7 +1134,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>83</v>
       </c>
@@ -1151,7 +1160,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>84</v>
       </c>
@@ -1177,7 +1186,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>85</v>
       </c>
@@ -1203,7 +1212,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>86</v>
       </c>
@@ -1225,9 +1234,11 @@
       <c r="G9" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="H9" s="10"/>
-    </row>
-    <row r="10" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H9" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>87</v>
       </c>
@@ -1249,9 +1260,11 @@
       <c r="G10" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="H10" s="10"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H10" s="10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
       <c r="B11" s="14"/>
       <c r="C11" s="19" t="s">
@@ -1269,9 +1282,11 @@
       <c r="G11" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="H11" s="10"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H11" s="10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="B12" s="14"/>
       <c r="C12" s="19" t="s">
@@ -1291,7 +1306,7 @@
       </c>
       <c r="H12" s="10"/>
     </row>
-    <row r="13" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="14"/>
       <c r="C13" s="19" t="s">
@@ -1311,7 +1326,7 @@
       </c>
       <c r="H13" s="10"/>
     </row>
-    <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="14"/>
       <c r="C14" s="19" t="s">
@@ -1331,7 +1346,7 @@
       </c>
       <c r="H14" s="10"/>
     </row>
-    <row r="15" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="14"/>
       <c r="C15" s="19" t="s">
@@ -1351,7 +1366,7 @@
       </c>
       <c r="H15" s="10"/>
     </row>
-    <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="B16" s="14"/>
       <c r="C16" s="19" t="s">
@@ -1371,7 +1386,7 @@
       </c>
       <c r="H16" s="10"/>
     </row>
-    <row r="17" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
       <c r="B17" s="14"/>
       <c r="C17" s="19" t="s">
@@ -1389,7 +1404,7 @@
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
     </row>
-    <row r="18" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="14"/>
       <c r="C18" s="19" t="s">
@@ -1405,7 +1420,7 @@
       <c r="G18" s="10"/>
       <c r="H18" s="10"/>
     </row>
-    <row r="19" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
       <c r="B19" s="14"/>
       <c r="C19" s="19" t="s">
@@ -1421,7 +1436,7 @@
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
     </row>
-    <row r="20" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
       <c r="B20" s="14"/>
       <c r="C20" s="19" t="s">
@@ -1437,7 +1452,7 @@
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
       <c r="B21" s="14"/>
       <c r="C21" s="19" t="s">
@@ -1453,7 +1468,7 @@
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
       <c r="B22" s="14"/>
       <c r="C22" s="19" t="s">
@@ -1469,7 +1484,7 @@
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
     </row>
-    <row r="23" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
       <c r="B23" s="14"/>
       <c r="C23" s="19" t="s">
@@ -1485,7 +1500,7 @@
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
     </row>
-    <row r="24" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Docuimentación - Actualización CU
Actualización C102
Creación C202
Actualización Nomenclaturas
</commit_message>
<xml_diff>
--- a/Nomenclaturas.xlsx
+++ b/Nomenclaturas.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Proyecto\LDS\Testify\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Valeria\Documents\Oslo\Testify\Testify\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF880239-8DDA-4E3E-B1F1-C2E79F9E5597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30" yWindow="0" windowWidth="9705" windowHeight="10185"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="148">
   <si>
     <t>Codigo</t>
   </si>
@@ -470,13 +469,22 @@
     <t>Informe de Revisión tecnica formal.</t>
   </si>
   <si>
-    <t>Resumen de Reunión 22</t>
+    <t>Consultar Escenario</t>
+  </si>
+  <si>
+    <t>Asignar Escenario</t>
+  </si>
+  <si>
+    <t>Adjuntar Documentos</t>
+  </si>
+  <si>
+    <t>Comentar Escenario</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1063,11 +1071,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1145,7 +1153,7 @@
         <v>128</v>
       </c>
       <c r="J2" s="23" t="s">
-        <v>27</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1177,7 +1185,7 @@
         <v>129</v>
       </c>
       <c r="J3" s="24" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1209,7 +1217,7 @@
         <v>130</v>
       </c>
       <c r="J4" s="24" t="s">
-        <v>31</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1241,7 +1249,7 @@
         <v>131</v>
       </c>
       <c r="J5" s="24" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1272,7 +1280,9 @@
       <c r="I6" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="J6" s="24"/>
+      <c r="J6" s="24" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">

</xml_diff>

<commit_message>
Documentación - Memoria de Testify
Se añade el documento de la Memoria de Testify correspondiente al equipo de desarrollo OSLO de la materia Laboratorio de desarrollo de software, se añade el nombre al documento de nomenclaturas.
</commit_message>
<xml_diff>
--- a/Nomenclaturas.xlsx
+++ b/Nomenclaturas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Proyecto\LDS\Testify\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E95CB9F0-5A88-440B-BFA9-E2DCCA1FE4AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4AF6C24-2465-4E62-AEDF-580695D09803}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="180">
   <si>
     <t>Plan de Proyecto</t>
   </si>
@@ -240,9 +240,6 @@
     <t>IN10</t>
   </si>
   <si>
-    <t>IN11</t>
-  </si>
-  <si>
     <t>IN12</t>
   </si>
   <si>
@@ -562,6 +559,12 @@
   </si>
   <si>
     <t>Manual de Usuario Testify</t>
+  </si>
+  <si>
+    <t>Memoria Testify Equipo OSLO</t>
+  </si>
+  <si>
+    <t>T10</t>
   </si>
 </sst>
 </file>
@@ -1207,8 +1210,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1232,54 +1235,54 @@
   <sheetData>
     <row r="1" spans="1:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="P1" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q1" s="25" t="s">
         <v>146</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D1" s="24" t="s">
-        <v>146</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="P1" s="25" t="s">
-        <v>146</v>
-      </c>
-      <c r="Q1" s="25" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="29.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>1</v>
@@ -1294,42 +1297,42 @@
         <v>41</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>24</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>24</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N2" s="4" t="s">
         <v>24</v>
       </c>
       <c r="P2" s="27" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="Q2" s="26" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B3" s="22" t="s">
         <v>153</v>
-      </c>
-      <c r="B3" s="22" t="s">
-        <v>154</v>
       </c>
       <c r="D3" s="14" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F3" s="16" t="s">
         <v>11</v>
@@ -1338,36 +1341,36 @@
         <v>42</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L3" s="4" t="s">
         <v>45</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="P3" s="27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="Q3" s="26" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D4" s="14" t="s">
         <v>3</v>
@@ -1379,45 +1382,45 @@
         <v>12</v>
       </c>
       <c r="G4" s="18" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I4" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="J4" s="4" t="s">
-        <v>93</v>
-      </c>
       <c r="K4" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="L4" s="4" t="s">
         <v>27</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="P4" s="27" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Q4" s="26" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F5" s="16" t="s">
         <v>13</v>
@@ -1426,40 +1429,40 @@
         <v>45</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="N5" s="4"/>
       <c r="P5" s="27" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Q5" s="26" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D6" s="14" t="s">
         <v>5</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F6" s="16" t="s">
         <v>14</v>
@@ -1468,19 +1471,19 @@
         <v>27</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="P6" s="27" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Q6" s="26" t="s">
         <v>27</v>
@@ -1488,10 +1491,10 @@
     </row>
     <row r="7" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>6</v>
@@ -1506,30 +1509,30 @@
         <v>67</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P7" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q7" s="26" t="s">
         <v>167</v>
-      </c>
-      <c r="Q7" s="26" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D8" s="14" t="s">
         <v>7</v>
@@ -1544,19 +1547,19 @@
         <v>68</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="P8" s="27" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="Q8" s="26" t="s">
         <v>24</v>
@@ -1579,25 +1582,25 @@
         <v>17</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="P9" s="27" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q9" s="26" t="s">
         <v>175</v>
-      </c>
-      <c r="Q9" s="26" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1617,31 +1620,29 @@
         <v>18</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="P10" s="27" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q10" s="26" t="s">
         <v>177</v>
       </c>
-      <c r="Q10" s="26" t="s">
-        <v>178</v>
-      </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>71</v>
-      </c>
+      <c r="A11" s="1"/>
       <c r="B11" s="22" t="s">
         <v>57</v>
       </c>
@@ -1655,26 +1656,30 @@
         <v>19</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="P11" s="27"/>
-      <c r="Q11" s="26"/>
+        <v>131</v>
+      </c>
+      <c r="P11" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q11" s="26" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B12" s="22" t="s">
         <v>58</v>
@@ -1689,16 +1694,16 @@
         <v>20</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L12" s="4"/>
       <c r="P12" s="27"/>
@@ -1706,7 +1711,7 @@
     </row>
     <row r="13" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B13" s="22" t="s">
         <v>59</v>
@@ -1715,22 +1720,22 @@
         <v>30</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F13" s="16" t="s">
         <v>46</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J13" s="4" t="s">
         <v>27</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="L13" s="4"/>
       <c r="P13" s="27"/>
@@ -1738,7 +1743,7 @@
     </row>
     <row r="14" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B14" s="22" t="s">
         <v>60</v>
@@ -1756,13 +1761,13 @@
         <v>45</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L14" s="4"/>
       <c r="P14" s="27"/>
@@ -1770,7 +1775,7 @@
     </row>
     <row r="15" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B15" s="22" t="s">
         <v>61</v>
@@ -1785,18 +1790,18 @@
         <v>48</v>
       </c>
       <c r="G15" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I15" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="J15" s="4" t="s">
         <v>170</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B16" s="22" t="s">
         <v>62</v>
@@ -1811,12 +1816,12 @@
         <v>49</v>
       </c>
       <c r="G16" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B17" s="22" t="s">
         <v>63</v>
@@ -1855,7 +1860,7 @@
         <v>43</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1865,7 +1870,7 @@
         <v>44</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>